<commit_message>
Test end to end Bank Loan with Pin
Test end to end using the last fuzzer version
</commit_message>
<xml_diff>
--- a/TestingTool_v3/Applications/C#Models/SimpleBankLoanCSharp/ConfigurationFile/Config.xlsx
+++ b/TestingTool_v3/Applications/C#Models/SimpleBankLoanCSharp/ConfigurationFile/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingTool_v2\TestModels\ConfigurationFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingTool_v3\Applications\C#Models\SimpleBankLoanCSharp\ConfigurationFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F02140C-35AD-447B-A81E-943C99643002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651E75D9-3FF3-42E8-B361-D4963CCD0C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="0" windowWidth="13824" windowHeight="7176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <t>testQueue</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v2</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool_v3</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v2\first.py</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool_v3\first.py</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v2\Applications\C#Models\SimpleBankLoanCSharp</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool_v3\Applications\C#Models\SimpleBankLoanCSharp</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
"Added time measurement for the testing pipeline in TestingTool_v3 for SimpleBankLoanCSharp"
</commit_message>
<xml_diff>
--- a/TestingTool_v3/Applications/C#Models/SimpleBankLoanCSharp/ConfigurationFile/Config.xlsx
+++ b/TestingTool_v3/Applications/C#Models/SimpleBankLoanCSharp/ConfigurationFile/Config.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingTool_v3\Applications\C#Models\SimpleBankLoanCSharp\ConfigurationFile\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651E75D9-3FF3-42E8-B361-D4963CCD0C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -51,9 +45,6 @@
     <t>*Full path of your python installation</t>
   </si>
   <si>
-    <t>C:\Users\adelinas\AppData\Local\Programs\Python\Python38</t>
-  </si>
-  <si>
     <t>ScriptWorkingFolder</t>
   </si>
   <si>
@@ -75,19 +66,22 @@
     <t>testQueue</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v3</t>
+    <t>C:\Users\Marina Cernat\Documents\GitHub\rpa-testing\TestingTool_v3</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v3\first.py</t>
+    <t>C:\Users\Marina Cernat\Documents\GitHub\rpa-testing\TestingTool_v3\first.py</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v3\Applications\C#Models\SimpleBankLoanCSharp</t>
+    <t>C:\Users\Marina Cernat\Documents\GitHub\rpa-testing\TestingTool_v3\Applications\C#Models\SimpleBankLoanCSharp</t>
+  </si>
+  <si>
+    <t>C:\Users\Marina Cernat\AppData\Local\Programs\Python\Python38</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -142,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -150,6 +144,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +257,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -456,26 +451,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="82.6640625" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="111.1796875" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -517,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -528,8 +523,8 @@
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
@@ -538,37 +533,37 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1570,19 +1565,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1619,7 +1614,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>